<commit_message>
Update captcha parameter to path & test malindo
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Portal_Malindoairways/Data/Config Prod.xlsx
+++ b/Traveloka_DataAutomation_Portal_Malindoairways/Data/Config Prod.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Malindoid\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Portal_Malindoairways\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A64B212-3D45-4DCD-A3C6-711F57AD6F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B1C3A6-2D6E-447C-AC59-BEAC9C60DE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="3360" windowWidth="21588" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="336" yWindow="336" windowWidth="19308" windowHeight="8640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -338,9 +338,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -378,7 +378,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -484,7 +484,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -626,7 +626,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -747,7 +747,10 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.3" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.3" customHeight="1">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+    </row>
     <row r="11" spans="1:26" ht="14.3" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.3" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.3" customHeight="1"/>
@@ -2909,8 +2912,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>

</xml_diff>